<commit_message>
"done with all updates"
</commit_message>
<xml_diff>
--- a/public/sample_departments.xlsx
+++ b/public/sample_departments.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C406498B-FC84-4577-A2E9-F327EF9AC9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="foodland" sheetId="1" r:id="rId1"/>
@@ -14,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>description</t>
   </si>
@@ -25,21 +23,9 @@
     <t>Responsible for product development and maintenance.</t>
   </si>
   <si>
-    <t>Engineering</t>
-  </si>
-  <si>
-    <t>Human Resources</t>
-  </si>
-  <si>
     <t>Manages employee relations and recruitment.</t>
   </si>
   <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
     <t>Handles advertising, campaigns, and promotions.</t>
   </si>
   <si>
@@ -49,20 +35,41 @@
     <t>Provides help and support to users.</t>
   </si>
   <si>
-    <t>Customer Support</t>
-  </si>
-  <si>
     <t>IT</t>
   </si>
   <si>
     <t>Responsible for product development and maintenance IT.</t>
+  </si>
+  <si>
+    <t>companyId</t>
+  </si>
+  <si>
+    <t>ef970b3d-5a2b-4b25-9b2e-c3b73d30a5c3</t>
+  </si>
+  <si>
+    <t>Customer Supports</t>
+  </si>
+  <si>
+    <t>Salesss</t>
+  </si>
+  <si>
+    <t>markl</t>
+  </si>
+  <si>
+    <t>Human Resourcesdd</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>ddss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +81,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -386,83 +399,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="64.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>